<commit_message>
Versión Web y Desktop Unificados
</commit_message>
<xml_diff>
--- a/mapGenerator/mapa-web.xlsx
+++ b/mapGenerator/mapa-web.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UPC_2024\MAS4CHICKEN\mapGenerator\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ca06b8c947122572/Documents/GitHub/MAS4CHICKEN/mapGenerator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BFC042-17E5-481B-B610-408CA549B46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{F9BFC042-17E5-481B-B610-408CA549B46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B59B61FE-51F4-4FAD-B3A4-635D461E0017}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -359,15 +359,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:CBL3"/>
+  <dimension ref="B1:CBL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CAJ1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:CBL3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:2092" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:2092" x14ac:dyDescent="0.3">
       <c r="B1">
         <v>-12</v>
       </c>
@@ -6642,7 +6642,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:2092" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:2092" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -10826,7 +10826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="2:2092" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:2092" x14ac:dyDescent="0.3">
       <c r="B3" t="str">
         <f>+B2&amp;B1</f>
         <v>[-12</v>
@@ -19190,6 +19190,12 @@
       <c r="CBL3" t="str">
         <f t="shared" ref="CBL3" si="1391">+CBL1&amp;CBL2</f>
         <v>0]</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2092" x14ac:dyDescent="0.3">
+      <c r="B6" t="str">
+        <f>_xlfn.TEXTJOIN(" ", FALSE, B1:CBL1)</f>
+        <v>-12 15 0 -11 15 0 -10 15 0 -9 15 0 -8 15 0 -7 15 0 -6 15 0 -5 15 0 -4 15 0 -3 15 0 -2 15 0 -1 15 0 0 15 0 1 15 0 2 15 0 3 15 0 4 15 0 5 15 0 6 15 0 7 15 0 8 15 0 9 15 0 10 15 0 11 15 0 -12 14 0 -11 14 0 -10 14 0 -9 14 0 -8 14 0 -7 14 0 -6 14 0 -5 14 0 -4 14 0 -3 14 0 -2 14 0 -1 14 0 0 14 0 1 14 0 2 14 0 3 14 0 4 14 0 5 14 0 6 14 0 7 14 0 8 14 0 9 14 0 10 14 0 11 14 0 -12 13 0 -11 13 0 -10 13 0 -9 13 0 -8 13 0 -7 13 0 -6 13 0 -5 13 0 -4 13 0 -3 13 0 -2 13 0 -1 13 0 0 13 0 1 13 0 2 13 0 3 13 0 4 13 0 5 13 0 6 13 0 7 13 0 8 13 0 9 13 0 10 13 0 11 13 0 -12 12 0 -11 12 0 -10 12 0 -9 12 0 -8 12 0 -7 12 0 -6 12 0 -5 12 0 -4 12 0 -3 12 0 -2 12 0 -1 12 27 0 12 0 1 12 0 2 12 0 3 12 0 4 12 0 5 12 0 6 12 0 7 12 0 8 12 0 9 12 0 10 12 0 11 12 0 12 12 0 -12 11 0 -11 11 45 -10 11 45 -9 11 45 -8 11 45 -7 11 45 -6 11 45 -5 11 45 -4 11 45 -3 11 45 -2 11 45 -1 11 45 0 11 45 1 11 45 2 11 45 3 11 45 4 11 45 5 11 45 6 11 45 7 11 45 8 11 45 9 11 45 10 11 45 11 11 45 12 11 0 -12 10 0 -11 10 45 -10 10 45 -9 10 35 -8 10 35 -7 10 45 -6 10 45 -5 10 35 -4 10 35 -3 10 45 -2 10 45 -1 10 35 0 10 35 1 10 45 2 10 45 3 10 35 4 10 35 5 10 45 6 10 45 7 10 35 8 10 35 9 10 45 10 10 45 11 10 45 12 10 0 -12 9 0 -11 9 45 -10 9 45 -9 9 45 -8 9 45 -7 9 45 -6 9 45 -5 9 45 -4 9 45 -3 9 45 -2 9 45 -1 9 45 0 9 45 1 9 45 2 9 45 3 9 45 4 9 45 5 9 45 6 9 45 7 9 45 8 9 45 9 9 45 10 9 45 11 9 45 12 9 0 -12 8 0 -11 8 45 -10 8 45 -9 8 45 -8 8 45 -7 8 45 -6 8 45 -5 8 45 -4 8 45 -3 8 45 -2 8 45 -1 8 45 0 8 45 1 8 45 2 8 45 3 8 45 4 8 45 5 8 45 6 8 45 7 8 45 8 8 45 9 8 45 10 8 45 11 8 45 12 8 0 -12 7 0 -11 7 45 -10 7 45 -9 7 35 -8 7 35 -7 7 45 -6 7 45 -5 7 35 -4 7 35 -3 7 45 -2 7 45 -1 7 35 0 7 35 1 7 45 2 7 45 3 7 35 4 7 35 5 7 45 6 7 45 7 7 35 8 7 35 9 7 45 10 7 45 11 7 45 12 7 0 -12 6 0 -11 6 45 -10 6 45 -9 6 45 -8 6 45 -7 6 45 -6 6 45 -5 6 45 -4 6 45 -3 6 45 -2 6 45 -1 6 45 0 6 45 1 6 45 2 6 45 3 6 45 4 6 45 5 6 45 6 6 45 7 6 45 8 6 45 9 6 45 10 6 45 11 6 45 12 6 0 -12 5 0 -11 5 45 -10 5 45 -9 5 45 -8 5 45 -7 5 45 -6 5 45 -5 5 45 -4 5 45 -3 5 45 -2 5 45 -1 5 45 0 5 45 1 5 45 2 5 45 3 5 45 4 5 45 5 5 45 6 5 45 7 5 45 8 5 45 9 5 45 10 5 45 11 5 45 12 5 0 -12 4 0 -11 4 45 -10 4 45 -9 4 35 -8 4 35 -7 4 45 -6 4 45 -5 4 35 -4 4 35 -3 4 45 -2 4 45 -1 4 35 0 4 35 1 4 45 2 4 45 3 4 35 4 4 35 5 4 45 6 4 45 7 4 35 8 4 35 9 4 45 10 4 45 11 4 45 12 4 0 -12 3 0 -11 3 45 -10 3 45 -9 3 45 -8 3 45 -7 3 45 -6 3 45 -5 3 45 -4 3 45 -3 3 45 -2 3 45 -1 3 45 0 3 45 1 3 45 2 3 45 3 3 45 4 3 45 5 3 45 6 3 45 7 3 45 8 3 45 9 3 45 10 3 45 11 3 45 12 3 0 -12 2 0 -11 2 45 -10 2 45 -9 2 45 -8 2 45 -7 2 45 -6 2 45 -5 2 45 -4 2 45 -3 2 45 -2 2 45 -1 2 45 0 2 45 1 2 45 2 2 45 3 2 45 4 2 45 5 2 45 6 2 45 7 2 45 8 2 45 9 2 45 10 2 45 11 2 45 12 2 0 -12 1 0 -11 1 45 -10 1 45 -9 1 35 -8 1 35 -7 1 45 -6 1 45 -5 1 35 -4 1 35 -3 1 45 -2 1 45 -1 1 35 0 1 35 1 1 45 2 1 45 3 1 35 4 1 35 5 1 45 6 1 45 7 1 35 8 1 35 9 1 45 10 1 45 11 1 45 12 1 0 -12 0 0 -11 0 45 -10 0 45 -9 0 45 -8 0 45 -7 0 45 -6 0 45 -5 0 45 -4 0 45 -3 0 45 -2 0 45 -1 0 45 0 0 45 1 0 45 2 0 45 3 0 45 4 0 45 5 0 45 6 0 45 7 0 45 8 0 45 9 0 45 10 0 45 11 0 45 12 0 0 -12 -1 0 -11 -1 45 -10 -1 45 -9 -1 45 -8 -1 45 -7 -1 45 -6 -1 45 -5 -1 45 -4 -1 45 -3 -1 45 -2 -1 45 -1 -1 45 0 -1 45 1 -1 45 2 -1 45 3 -1 45 4 -1 45 5 -1 45 6 -1 45 7 -1 45 8 -1 45 9 -1 45 10 -1 45 11 -1 45 12 -1 0 -12 -2 0 -11 -2 45 -10 -2 45 -9 -2 35 -8 -2 35 -7 -2 45 -6 -2 45 -5 -2 35 -4 -2 35 -3 -2 45 -2 -2 45 -1 -2 35 0 -2 35 1 -2 45 2 -2 45 3 -2 35 4 -2 35 5 -2 45 6 -2 45 7 -2 35 8 -2 35 9 -2 45 10 -2 45 11 -2 45 12 -2 0 -12 -3 0 -11 -3 45 -10 -3 45 -9 -3 45 -8 -3 45 -7 -3 45 -6 -3 45 -5 -3 45 -4 -3 45 -3 -3 45 -2 -3 45 -1 -3 45 0 -3 45 1 -3 45 2 -3 45 3 -3 45 4 -3 45 5 -3 45 6 -3 45 7 -3 45 8 -3 45 9 -3 45 10 -3 45 11 -3 45 12 -3 0 -12 -4 0 -11 -4 45 -10 -4 45 -9 -4 45 -8 -4 45 -7 -4 45 -6 -4 45 -5 -4 45 -4 -4 45 -3 -4 45 -2 -4 45 -1 -4 45 0 -4 45 1 -4 45 2 -4 45 3 -4 45 4 -4 45 5 -4 45 6 -4 45 7 -4 45 8 -4 45 9 -4 45 10 -4 45 11 -4 45 12 -4 0 -12 -5 0 -11 -5 45 -10 -5 45 -9 -5 45 -8 -5 45 -7 -5 45 -6 -5 45 -5 -5 45 -4 -5 45 -3 -5 45 -2 -5 45 -1 -5 45 0 -5 45 1 -5 45 2 -5 45 3 -5 45 4 -5 45 5 -5 45 6 -5 45 7 -5 45 8 -5 45 9 -5 45 10 -5 45 11 -5 45 12 -5 0 -12 -6 0 -11 -6 0 -10 -6 0 -9 -6 0 -8 -6 0 -7 -6 0 -6 -6 0 -5 -6 0 -4 -6 5 -3 -6 5 -2 -6 5 -1 -6 0 0 -6 0 1 -6 0 2 -6 0 3 -6 0 4 -6 0 5 -6 0 6 -6 0 7 -6 0 8 -6 0 9 -6 0 10 -6 0 11 -6 0 12 -6 0 -12 -7 0 -11 -7 5 -10 -7 5 -9 -7 5 -8 -7 5 -7 -7 5 -6 -7 5 -5 -7 5 -4 -7 5 -3 -7 5 -2 -7 5 -1 -7 5 0 -7 4 1 -7 4 2 -7 4 3 -7 4 4 -7 4 5 -7 4 6 -7 4 7 -7 4 8 -7 4 9 -7 4 10 -7 4 11 -7 4 12 -7 0 -12 -8 0 -11 -8 5 -10 -8 5 -9 -8 5 -8 -8 5 -7 -8 5 -6 -8 5 -5 -8 5 -4 -8 5 -3 -8 5 -2 -8 5 -1 -8 5 0 -8 4 1 -8 4 2 -8 4 3 -8 4 4 -8 4 5 -8 4 6 -8 4 7 -8 4 8 -8 4 9 -8 4 10 -8 4 11 -8 4 12 -8 0 -12 -9 0 -11 -9 5 -10 -9 5 -9 -9 5 -8 -9 5 -7 -9 5 -6 -9 5 -5 -9 5 -4 -9 5 -3 -9 5 -2 -9 5 -1 -9 5 0 -9 4 1 -9 4 2 -9 4 3 -9 4 4 -9 4 5 -9 4 6 -9 4 7 -9 4 8 -9 4 9 -9 4 10 -9 4 11 -9 4 12 -9 0 -12 -10 0 -11 -10 5 -10 -10 5 -9 -10 5 -8 -10 5 -7 -10 5 -6 -10 5 -5 -10 5 -4 -10 5 -3 -10 5 -2 -10 5 -1 -10 5 0 -10 4 1 -10 4 2 -10 4 3 -10 4 4 -10 4 5 -10 4 6 -10 4 7 -10 4 8 -10 4 9 -10 4 10 -10 4 11 -10 4 12 -10 0 -12 -11 0 -11 -11 5 -10 -11 5 -9 -11 5 -8 -11 5 -7 -11 5 -6 -11 5 -5 -11 5 -4 -11 5 -3 -11 5 -2 -11 5 -1 -11 5 0 -11 4 1 -11 4 2 -11 4 3 -11 4 4 -11 4 5 -11 4 6 -11 4 7 -11 4 8 -11 4 9 -11 4 10 -11 4 11 -11 4 12 -11 0 -12 -12 0 -11 -12 0 -10 -12 0 -9 -12 0 -8 -12 0 -7 -12 0 -6 -12 0 -5 -12 0 -4 -12 0 -3 -12 0 -2 -12 0 -1 -12 0 0 -12 0 1 -12 0 2 -12 0 3 -12 0 4 -12 0 5 -12 0 6 -12 0 7 -12 0 8 -12 0 9 -12 0 10 -12 0 11 -12 0 12 -12 0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>